<commit_message>
Add css and fixed the ui.
</commit_message>
<xml_diff>
--- a/uploads/sample.xlsx
+++ b/uploads/sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="17540" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="linear problem" sheetId="2" r:id="rId1"/>
@@ -59,10 +59,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>unit</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>min</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -129,6 +125,10 @@
   </si>
   <si>
     <t>b9</t>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -539,34 +539,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -824,7 +824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -837,15 +837,15 @@
     <row r="1" spans="1:3">
       <c r="A1" s="3"/>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2">
         <v>200</v>
@@ -856,7 +856,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2">
         <v>75</v>
@@ -867,7 +867,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2">
         <v>5</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2">
         <v>10</v>
@@ -889,7 +889,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2">
         <v>50</v>
@@ -900,7 +900,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2">
         <v>5</v>
@@ -922,7 +922,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2">
         <v>25</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1">
         <v>12</v>

</xml_diff>